<commit_message>
agregaAutorizado + sq_cliente y sq_persona
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ABD\ABD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A32702A-08D9-4E32-91FD-83EB46AA327B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>Nombre del Grupo: JARD</t>
   </si>
@@ -281,11 +280,17 @@
   <si>
     <t>comprobar si funciona RF8</t>
   </si>
+  <si>
+    <t>falta revisar</t>
+  </si>
+  <si>
+    <t>faltar P_cobro</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -692,7 +697,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Hoja2-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Hoja2-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -710,9 +715,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Columna1"/>
+    <tableColumn id="1" name="Columna1"/>
   </tableColumns>
   <tableStyleInfo name="Hoja2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -915,29 +920,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="57.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="51.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14.4">
       <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
@@ -967,7 +972,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="14.4">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -999,7 +1004,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="28.8">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="14.4">
       <c r="A5" s="11">
         <v>1</v>
       </c>
@@ -1054,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="30">
+    <row r="6" spans="1:26" ht="28.8">
       <c r="B6" s="16"/>
       <c r="C6" s="17" t="s">
         <v>14</v>
@@ -1068,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="30">
+    <row r="7" spans="1:26" ht="28.8">
       <c r="B7" s="20"/>
       <c r="C7" s="21" t="s">
         <v>16</v>
@@ -1082,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30">
+    <row r="8" spans="1:26" ht="28.8">
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
         <v>17</v>
@@ -1100,7 +1105,7 @@
       </c>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="14.4">
       <c r="A9" s="11">
         <f>A5+1</f>
         <v>2</v>
@@ -1113,7 +1118,7 @@
       <c r="E9" s="26"/>
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="14.4">
       <c r="B10" s="60"/>
       <c r="C10" s="27" t="s">
         <v>20</v>
@@ -1126,39 +1131,48 @@
         <f t="shared" ref="F10:F12" si="1">IF(D10="NO",0,1)</f>
         <v>1</v>
       </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
       <c r="I10" s="24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="14.4">
       <c r="B11" s="61"/>
       <c r="C11" s="22" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.4">
       <c r="B12" s="61"/>
       <c r="C12" s="22" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="30">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="28.8">
       <c r="B13" s="62"/>
       <c r="C13" s="30" t="s">
         <v>25</v>
@@ -1171,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="14.4">
       <c r="A14" s="31">
         <f>A9+1</f>
         <v>3</v>
@@ -1184,7 +1198,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="14.4">
       <c r="A15" s="6"/>
       <c r="B15" s="33"/>
       <c r="C15" s="20" t="s">
@@ -1223,7 +1237,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" ht="14.4">
       <c r="B16" s="20"/>
       <c r="C16" s="34" t="s">
         <v>29</v>
@@ -1240,14 +1254,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="14.4">
       <c r="B17" s="20"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
       <c r="E17" s="22"/>
       <c r="F17" s="35"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="31">
         <f>A14+1</f>
         <v>4</v>
@@ -1260,7 +1274,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="35"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="14.4">
       <c r="B19" s="20"/>
       <c r="C19" s="34" t="s">
         <v>32</v>
@@ -1277,7 +1291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="14.4">
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="39"/>
@@ -1303,12 +1317,15 @@
         <v>35</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="19">
         <f>IF(D22="NO",0,1)</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
       </c>
       <c r="I22" s="24" t="s">
         <v>33</v>
@@ -1350,6 +1367,9 @@
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="19"/>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
       <c r="K26" s="24" t="s">
         <v>69</v>
       </c>
@@ -1505,7 +1525,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6">
         <f>SUM(F5:F33)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -6801,7 +6821,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja2!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -6814,28 +6834,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="26" width="10.7109375" customWidth="1"/>
+    <col min="2" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="14.4">
       <c r="A1" s="56" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="14.4">
       <c r="A2" s="56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="14.4">
       <c r="A3" s="56" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Rubrica actualizada con V_VISTAS
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ABD\ABD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73568CD6-B02D-4AAA-81A5-C89C75370EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="2595" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>Nombre del Grupo: JARD</t>
   </si>
@@ -286,11 +287,14 @@
   <si>
     <t>ultimo vistazo por si falta controlar algo</t>
   </si>
+  <si>
+    <t>FUNCIONAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -357,7 +361,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +378,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -532,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -660,6 +670,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -672,9 +685,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,7 +717,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Hoja2-style" pivot="0" count="3">
+    <tableStyle name="Hoja2-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -724,9 +735,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:A3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
-    <tableColumn id="1" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Columna1"/>
   </tableColumns>
   <tableStyleInfo name="Hoja2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -929,38 +940,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="57.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
-    <col min="12" max="26" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.4">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:26">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -981,7 +992,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.4">
+    <row r="2" spans="1:26">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -990,13 +1001,13 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1013,7 +1024,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="28.8">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +1053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1053,7 +1064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="5" spans="1:26">
       <c r="A5" s="11">
         <v>1</v>
       </c>
@@ -1068,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="28.8">
+    <row r="6" spans="1:26" ht="30">
       <c r="B6" s="16"/>
       <c r="C6" s="17" t="s">
         <v>14</v>
@@ -1082,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="28.8">
+    <row r="7" spans="1:26" ht="30">
       <c r="B7" s="20"/>
       <c r="C7" s="21" t="s">
         <v>16</v>
@@ -1096,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="28.8">
+    <row r="8" spans="1:26" ht="30">
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
         <v>17</v>
@@ -1114,7 +1125,7 @@
       </c>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:26" ht="14.4">
+    <row r="9" spans="1:26">
       <c r="A9" s="11">
         <f>A5+1</f>
         <v>2</v>
@@ -1127,8 +1138,8 @@
       <c r="E9" s="26"/>
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:26" ht="14.4">
-      <c r="B10" s="60"/>
+    <row r="10" spans="1:26">
+      <c r="B10" s="61"/>
       <c r="C10" s="27" t="s">
         <v>20</v>
       </c>
@@ -1140,15 +1151,15 @@
         <f t="shared" ref="F10:F12" si="1">IF(D10="NO",0,1)</f>
         <v>1</v>
       </c>
-      <c r="G10" t="s">
-        <v>70</v>
-      </c>
       <c r="I10" s="24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.4">
-      <c r="B11" s="61"/>
+      <c r="K10" s="64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="B11" s="62"/>
       <c r="C11" s="22" t="s">
         <v>22</v>
       </c>
@@ -1164,8 +1175,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.4">
-      <c r="B12" s="61"/>
+    <row r="12" spans="1:26">
+      <c r="B12" s="62"/>
       <c r="C12" s="22" t="s">
         <v>24</v>
       </c>
@@ -1181,8 +1192,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="28.8">
-      <c r="B13" s="62"/>
+    <row r="13" spans="1:26" ht="30">
+      <c r="B13" s="63"/>
       <c r="C13" s="30" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.4">
+    <row r="14" spans="1:26">
       <c r="A14" s="31">
         <f>A9+1</f>
         <v>3</v>
@@ -1204,10 +1215,10 @@
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="63"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:26" ht="14.4">
+    <row r="15" spans="1:26">
       <c r="A15" s="6"/>
       <c r="B15" s="33"/>
       <c r="C15" s="20" t="s">
@@ -1246,7 +1257,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26" ht="14.4">
+    <row r="16" spans="1:26">
       <c r="B16" s="20"/>
       <c r="C16" s="34" t="s">
         <v>28</v>
@@ -1263,14 +1274,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.4">
+    <row r="17" spans="1:11">
       <c r="B17" s="20"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
       <c r="E17" s="22"/>
       <c r="F17" s="35"/>
     </row>
-    <row r="18" spans="1:11" ht="14.4">
+    <row r="18" spans="1:11">
       <c r="A18" s="31">
         <f>A14+1</f>
         <v>4</v>
@@ -1283,7 +1294,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="35"/>
     </row>
-    <row r="19" spans="1:11" ht="14.4">
+    <row r="19" spans="1:11">
       <c r="B19" s="20"/>
       <c r="C19" s="34" t="s">
         <v>31</v>
@@ -1300,7 +1311,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.4">
+    <row r="20" spans="1:11">
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="39"/>
@@ -6830,7 +6841,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Hoja2!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -6843,28 +6854,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="26" width="10.6640625" customWidth="1"/>
+    <col min="2" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.4">
+    <row r="1" spans="1:1">
       <c r="A1" s="56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.4">
+    <row r="2" spans="1:1">
       <c r="A2" s="56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.4">
+    <row r="3" spans="1:1">
       <c r="A3" s="56" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
añadido EJ2C y rubrica a color
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\ABD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5193A2AB-DA6C-4E46-BD72-7849C955A40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDACB53E-0DD9-4EE3-87F0-02B034DF3AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2595" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>Nombre del Grupo: JARD</t>
   </si>
@@ -301,6 +301,18 @@
   </si>
   <si>
     <t>En J_LIQUIDAR</t>
+  </si>
+  <si>
+    <t>LEYENDA COLORES:</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>HACER PRUEBAS:</t>
+  </si>
+  <si>
+    <t>TERMINAR:</t>
   </si>
 </sst>
 </file>
@@ -381,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,8 +412,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -552,11 +576,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -619,16 +658,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -685,6 +718,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -697,10 +737,46 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="J19" sqref="J18:J19"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -970,7 +1046,7 @@
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" customWidth="1"/>
     <col min="8" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" customWidth="1"/>
@@ -978,15 +1054,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1016,13 +1092,13 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1075,7 +1151,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="4"/>
-      <c r="J4" s="64"/>
+      <c r="J4" s="57"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="10">
@@ -1094,7 +1170,7 @@
     </row>
     <row r="6" spans="1:26" ht="30">
       <c r="B6" s="15"/>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="65" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -1110,7 +1186,7 @@
     </row>
     <row r="7" spans="1:26" ht="30">
       <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="66" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -1126,7 +1202,7 @@
     </row>
     <row r="8" spans="1:26" ht="30">
       <c r="B8" s="19"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="67" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1158,11 +1234,11 @@
       <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="B10" s="61"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="62"/>
+      <c r="C10" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="19" t="s">
@@ -1175,16 +1251,16 @@
       <c r="I10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="57" t="s">
+      <c r="K10" s="55" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="B11" s="62"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="63"/>
+      <c r="C11" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="19"/>
@@ -1197,11 +1273,11 @@
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="B12" s="62"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="63"/>
+      <c r="C12" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="19"/>
@@ -1214,8 +1290,8 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="30">
-      <c r="B13" s="63"/>
-      <c r="C13" s="29" t="s">
+      <c r="B13" s="64"/>
+      <c r="C13" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1227,39 +1303,39 @@
       </c>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="30">
+      <c r="A14" s="28">
         <f>A9+1</f>
         <v>3</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="31"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="56"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="6"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="34">
+      <c r="F15" s="32">
         <f t="shared" ref="F15:F16" si="2">IF(D15="NO",0,1)</f>
         <v>1</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="33" t="s">
         <v>71</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="35" t="s">
+      <c r="K15" s="33" t="s">
         <v>68</v>
       </c>
       <c r="L15" s="6"/>
@@ -1280,14 +1356,14 @@
     </row>
     <row r="16" spans="1:26">
       <c r="B16" s="19"/>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="31" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="21"/>
-      <c r="F16" s="34">
+      <c r="F16" s="32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1300,30 +1376,30 @@
     </row>
     <row r="17" spans="1:11">
       <c r="B17" s="19"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="34"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="30">
+      <c r="A18" s="28">
         <f>A14+1</f>
         <v>4</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="28"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="34"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:11">
       <c r="B19" s="19"/>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="36" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="4"/>
@@ -1331,37 +1407,37 @@
         <f>IF(D19="NO",0,1)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="65"/>
+      <c r="G19" s="58"/>
       <c r="I19" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="38"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="4"/>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="30">
+      <c r="A21" s="28">
         <f>A18+1</f>
         <v>5</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="20"/>
       <c r="E21" s="4"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="B22" s="19"/>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="36" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="4"/>
@@ -1378,33 +1454,33 @@
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="38"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="4"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="21"/>
       <c r="E24" s="4"/>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="30">
+      <c r="A25" s="28">
         <v>5</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="39"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="20"/>
       <c r="E25" s="4"/>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="B26" s="19"/>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="71" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="17" t="s">
@@ -1423,29 +1499,29 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="38"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="36"/>
       <c r="E27" s="4"/>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="30">
+      <c r="A28" s="28">
         <f>A25+1</f>
         <v>6</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="34"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="32"/>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:11" ht="31.5" customHeight="1">
-      <c r="B29" s="32"/>
-      <c r="C29" s="19" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="36" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="4"/>
@@ -1455,24 +1531,24 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="30">
+      <c r="A30" s="28">
         <f>A28+1</f>
         <v>7</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="40"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="4"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B31" s="32"/>
-      <c r="C31" s="19" t="s">
+      <c r="B31" s="30"/>
+      <c r="C31" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="36" t="s">
         <v>22</v>
       </c>
       <c r="E31" s="4"/>
@@ -1482,57 +1558,65 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B32" s="41"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="4"/>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="30">
+      <c r="A33" s="28">
         <f>A30+1</f>
         <v>8</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44" t="s">
+      <c r="C33" s="75"/>
+      <c r="D33" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="43"/>
-      <c r="F33" s="45">
+      <c r="E33" s="41"/>
+      <c r="F33" s="43">
         <f>IF(D33="NO",0,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="6"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="47"/>
-      <c r="Q34" s="47"/>
-      <c r="R34" s="47"/>
-      <c r="S34" s="47"/>
-      <c r="T34" s="47"/>
-      <c r="U34" s="47"/>
-      <c r="V34" s="47"/>
-      <c r="W34" s="47"/>
-      <c r="X34" s="47"/>
-      <c r="Y34" s="47"/>
-      <c r="Z34" s="47"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" s="78"/>
+      <c r="J34" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" s="79"/>
+      <c r="L34" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="M34" s="80"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="6"/>
@@ -1564,7 +1648,7 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="46" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="4"/>
@@ -1596,38 +1680,38 @@
       <c r="Z36" s="6"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="47"/>
-      <c r="B37" s="49" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="47"/>
-      <c r="N37" s="47"/>
-      <c r="O37" s="47"/>
-      <c r="P37" s="47"/>
-      <c r="Q37" s="47"/>
-      <c r="R37" s="47"/>
-      <c r="S37" s="47"/>
-      <c r="T37" s="47"/>
-      <c r="U37" s="47"/>
-      <c r="V37" s="47"/>
-      <c r="W37" s="47"/>
-      <c r="X37" s="47"/>
-      <c r="Y37" s="47"/>
-      <c r="Z37" s="47"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="6"/>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="46" t="s">
         <v>43</v>
       </c>
       <c r="C38" s="4"/>
@@ -1718,10 +1802,10 @@
       <c r="B41" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="51"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="49"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -1749,7 +1833,7 @@
       <c r="C42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="4"/>
@@ -1784,7 +1868,7 @@
       <c r="C43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E43" s="4"/>
@@ -1818,7 +1902,7 @@
       <c r="C44" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E44" s="4"/>
@@ -1833,7 +1917,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
-      <c r="F45" s="52"/>
+      <c r="F45" s="50"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -1860,7 +1944,7 @@
         <f>A41+1</f>
         <v>2</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="30" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="4"/>
@@ -1894,7 +1978,7 @@
       <c r="C47" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="28" t="s">
+      <c r="D47" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E47" s="4"/>
@@ -1929,7 +2013,7 @@
       <c r="C48" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="D48" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="4"/>
@@ -1959,7 +2043,7 @@
       <c r="Z48" s="6"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="30">
+      <c r="A49" s="28">
         <f>A46+1</f>
         <v>3</v>
       </c>
@@ -1976,7 +2060,7 @@
       <c r="C50" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="D50" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E50" s="4"/>
@@ -1990,7 +2074,7 @@
       <c r="C51" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D51" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E51" s="4"/>
@@ -2004,7 +2088,7 @@
       <c r="C52" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="28"/>
+      <c r="D52" s="27"/>
       <c r="E52" s="4"/>
       <c r="F52" s="18"/>
     </row>
@@ -2013,7 +2097,7 @@
       <c r="C53" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D53" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E53" s="4"/>
@@ -2027,7 +2111,7 @@
       <c r="C54" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E54" s="4"/>
@@ -2041,7 +2125,7 @@
       <c r="C55" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E55" s="4"/>
@@ -2055,7 +2139,7 @@
       <c r="C56" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D56" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E56" s="4"/>
@@ -2079,11 +2163,11 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A58" s="30">
+      <c r="A58" s="28">
         <f>A49+1</f>
         <v>4</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C58" s="4"/>
@@ -2093,10 +2177,10 @@
     </row>
     <row r="59" spans="1:6" ht="30.75" customHeight="1">
       <c r="B59" s="19"/>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="28" t="s">
+      <c r="D59" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -2108,18 +2192,18 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B60" s="32"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A61" s="30">
+      <c r="A61" s="28">
         <f>A58+1</f>
         <v>5</v>
       </c>
-      <c r="B61" s="53" t="s">
+      <c r="B61" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C61" s="3"/>
@@ -2132,7 +2216,7 @@
       <c r="C62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E62" s="4"/>
@@ -2146,7 +2230,7 @@
       <c r="C63" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E63" s="4"/>
@@ -2161,7 +2245,7 @@
       <c r="C64" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="28" t="s">
+      <c r="D64" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E64" s="4"/>
@@ -2171,15 +2255,15 @@
     </row>
     <row r="65" spans="1:6" ht="32.25" customHeight="1">
       <c r="A65" s="4"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="43" t="s">
+      <c r="B65" s="40"/>
+      <c r="C65" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D65" s="54" t="s">
+      <c r="D65" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E65" s="43"/>
-      <c r="F65" s="45">
+      <c r="E65" s="41"/>
+      <c r="F65" s="43">
         <v>0</v>
       </c>
     </row>
@@ -6895,17 +6979,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="53" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios a nivel fisico rubrica casi completa
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC21AA85-274D-4379-86A8-1EBE99996A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC19A1F-BB5C-42EE-A10D-67CF762707DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2595" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -595,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -728,31 +728,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -763,6 +748,9 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -777,7 +765,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1037,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1057,15 +1051,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1095,13 +1089,13 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="77" t="s">
+      <c r="G2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1205,7 +1199,7 @@
     </row>
     <row r="8" spans="1:26" ht="30">
       <c r="B8" s="19"/>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="60" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1237,8 +1231,8 @@
       <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="B10" s="78"/>
-      <c r="C10" s="62" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="61" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="26" t="s">
@@ -1259,8 +1253,8 @@
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="B11" s="79"/>
-      <c r="C11" s="74" t="s">
+      <c r="B11" s="75"/>
+      <c r="C11" s="69" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="27" t="s">
@@ -1276,8 +1270,8 @@
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="B12" s="79"/>
-      <c r="C12" s="74" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="69" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="27" t="s">
@@ -1293,8 +1287,8 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="30">
-      <c r="B13" s="80"/>
-      <c r="C13" s="63" t="s">
+      <c r="B13" s="76"/>
+      <c r="C13" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1321,7 +1315,7 @@
     <row r="15" spans="1:26">
       <c r="A15" s="6"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="63" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="31" t="s">
@@ -1359,7 +1353,7 @@
     </row>
     <row r="16" spans="1:26">
       <c r="B16" s="19"/>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="62" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
@@ -1399,7 +1393,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="B19" s="19"/>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="70" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="36" t="s">
@@ -1437,7 +1431,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="B22" s="19"/>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="63" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="36" t="s">
@@ -1483,7 +1477,7 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="B26" s="19"/>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="63" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="17" t="s">
@@ -1521,7 +1515,7 @@
     </row>
     <row r="29" spans="1:11" ht="31.5" customHeight="1">
       <c r="B29" s="30"/>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="63" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="36" t="s">
@@ -1548,7 +1542,7 @@
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="B31" s="30"/>
-      <c r="C31" s="67" t="s">
+      <c r="C31" s="63" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="36" t="s">
@@ -1575,7 +1569,7 @@
       <c r="B33" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="42" t="s">
         <v>22</v>
       </c>
@@ -1592,21 +1586,21 @@
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
       <c r="F34" s="44"/>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="I34" s="71"/>
-      <c r="J34" s="70" t="s">
+      <c r="I34" s="66"/>
+      <c r="J34" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="K34" s="72"/>
-      <c r="L34" s="70" t="s">
+      <c r="K34" s="67"/>
+      <c r="L34" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="M34" s="73"/>
+      <c r="M34" s="68"/>
       <c r="N34" s="45"/>
       <c r="O34" s="45"/>
       <c r="P34" s="45"/>
@@ -2060,16 +2054,16 @@
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
       <c r="B50" s="19"/>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="79" t="s">
         <v>51</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="18">
         <f t="shared" ref="F50:F51" si="5">IF(D50="NO",0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
@@ -2180,7 +2174,7 @@
     </row>
     <row r="59" spans="1:6" ht="30.75" customHeight="1">
       <c r="B59" s="19"/>
-      <c r="C59" s="69" t="s">
+      <c r="C59" s="64" t="s">
         <v>60</v>
       </c>
       <c r="D59" s="27" t="s">

</xml_diff>